<commit_message>
antes de gemini disenando
</commit_message>
<xml_diff>
--- a/database/imlLibro1.xlsx
+++ b/database/imlLibro1.xlsx
@@ -5,10 +5,10 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\alejo\Downloads\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\laragon\www\mar\database\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E1C3A237-A806-4060-B6A4-3E55F9FC848A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9284E69C-191C-47E6-87A8-4831EE3DBFF3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-180" yWindow="-180" windowWidth="29160" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -1914,14 +1914,14 @@
   <dimension ref="A1:H124"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
-      <selection activeCell="E9" sqref="E9"/>
+      <selection activeCell="C1" sqref="C1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="12" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="11.5703125" style="1" customWidth="1"/>
     <col min="2" max="2" width="20.85546875" style="1" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="11.42578125" style="1"/>
+    <col min="3" max="3" width="21.85546875" style="1" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="32.140625" style="1" customWidth="1"/>
     <col min="5" max="5" width="15.140625" style="1" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="11.42578125" style="1"/>

</xml_diff>